<commit_message>
ssr Signed-off-by: wakaka2333 <kaka821581232@gmail.com>
</commit_message>
<xml_diff>
--- a/秋招公司投递情况及其进展.xlsx
+++ b/秋招公司投递情况及其进展.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
   <si>
     <t>公司名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +58,26 @@
   </si>
   <si>
     <t>面试完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>招银网络科技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>腾讯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简历投递</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简历投递</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -88,7 +108,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +118,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,12 +140,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,17 +431,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A17" sqref="A17:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -457,6 +486,193 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>